<commit_message>
changed general parameter to dictionary
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,21 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FB5289-8423-4A49-A801-2162638A9E01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F292C12F-6B30-4337-83A3-885B48F15A64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
     <sheet name="General Data" sheetId="5" r:id="rId2"/>
     <sheet name="Costs new investments" sheetId="16" r:id="rId3"/>
-    <sheet name="Costs of default system" sheetId="17" r:id="rId4"/>
+    <sheet name="Costs default system" sheetId="17" r:id="rId4"/>
     <sheet name="Demand" sheetId="13" r:id="rId5"/>
     <sheet name="Irradiation and temperatur" sheetId="15" r:id="rId6"/>
     <sheet name="irradiation_winter" sheetId="12" r:id="rId7"/>
-    <sheet name="Tabelle2" sheetId="18" r:id="rId8"/>
-    <sheet name="Tabelle1" sheetId="14" r:id="rId9"/>
-    <sheet name="Tabelle3" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>PV</t>
   </si>
@@ -90,9 +87,6 @@
     <t>Insulation</t>
   </si>
   <si>
-    <t>Charging_Station</t>
-  </si>
-  <si>
     <t>c_inv [€/kWp,m²,psc]</t>
   </si>
   <si>
@@ -180,12 +174,6 @@
     <t>n_household</t>
   </si>
   <si>
-    <t>Number of charging stations</t>
-  </si>
-  <si>
-    <t>n_charging_stations_total</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -198,9 +186,6 @@
     <t>Depreciation time</t>
   </si>
   <si>
-    <t>DOW p.P.</t>
-  </si>
-  <si>
     <t>Temperature heating</t>
   </si>
   <si>
@@ -246,15 +231,6 @@
     <t>Capacity Battery Car</t>
   </si>
   <si>
-    <t>investment</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>what contractor?</t>
-  </si>
-  <si>
     <t>Self financed</t>
   </si>
   <si>
@@ -264,9 +240,6 @@
     <t>Battery Powerflow</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>Charging Station</t>
   </si>
   <si>
@@ -280,6 +253,18 @@
   </si>
   <si>
     <t xml:space="preserve">Unit </t>
+  </si>
+  <si>
+    <t>Cost type default</t>
+  </si>
+  <si>
+    <t>DHW p.P.</t>
+  </si>
+  <si>
+    <t>Number of cars</t>
+  </si>
+  <si>
+    <t>n_cars_total</t>
   </si>
 </sst>
 </file>
@@ -659,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,41 +659,47 @@
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -719,13 +710,16 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -733,13 +727,16 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -747,69 +744,72 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -860,18 +860,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B89A9E0-155D-4689-B8B8-FE96A05CE183}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -881,7 +869,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,21 +884,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
       </c>
       <c r="C2">
         <v>0.02</v>
@@ -918,10 +906,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -951,10 +939,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>0.5</v>
@@ -962,10 +950,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
       </c>
       <c r="C7">
         <v>0.45</v>
@@ -973,10 +961,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>70</v>
@@ -984,10 +972,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>22</v>
@@ -995,10 +983,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -1006,10 +994,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>60</v>
@@ -1017,10 +1005,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>0.8</v>
@@ -1028,10 +1016,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>0.8</v>
@@ -1039,10 +1027,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1050,10 +1038,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -1061,10 +1049,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>60</v>
@@ -1072,10 +1060,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
       </c>
       <c r="C17">
         <v>0.2</v>
@@ -1106,47 +1094,47 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1166,7 +1154,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1186,7 +1174,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1206,7 +1194,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1226,10 +1214,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>2000</v>
@@ -1246,10 +1234,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -1266,10 +1254,10 @@
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4">
         <v>1500</v>
@@ -1376,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <f ca="1">'Costs new investments'!C14*0.1</f>
@@ -1398,7 +1386,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <f ca="1">'Costs new investments'!C15*0.1</f>
@@ -1420,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C16">
         <f ca="1">'Costs new investments'!C16*0.1</f>
@@ -1444,40 +1432,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429933C5-DFD0-42DC-9288-AD78420EFB5D}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1485,75 +1469,63 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B4">
         <v>200</v>
       </c>
-      <c r="D3">
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="D4">
         <v>0.2</v>
       </c>
-      <c r="F3">
+      <c r="E4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="D4">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="D5">
         <v>0.2</v>
       </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>200</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
       <c r="E5">
-        <v>0.2</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
@@ -1566,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1578,19 +1550,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2023,13 +1995,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -2745,414 +2717,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C5B1FE-1E76-4968-8384-D485CE54D1EC}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C0EF88-4887-4CA9-BA39-40AB3A7CB900}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed cost parameter to dictionary
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F292C12F-6B30-4337-83A3-885B48F15A64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C05E54-8EE7-4979-9DA6-AA14A27C6C02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>PV</t>
   </si>
@@ -258,13 +258,16 @@
     <t>Cost type default</t>
   </si>
   <si>
-    <t>DHW p.P.</t>
-  </si>
-  <si>
     <t>Number of cars</t>
   </si>
   <si>
     <t>n_cars_total</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Specific DHW</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,9 +660,10 @@
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -678,8 +682,11 @@
       <c r="F1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -698,8 +705,11 @@
       <c r="F2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -718,8 +728,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -735,8 +748,11 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -749,8 +765,11 @@
       <c r="F5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -758,7 +777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -766,7 +785,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -774,42 +793,42 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -868,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,7 +958,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1038,10 +1057,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -1538,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1983,12 +2002,12 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
investment and service cost to obj
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C05E54-8EE7-4979-9DA6-AA14A27C6C02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B922E7-CD95-479F-BFAB-CF7B7CD4BB63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>PV</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>Specific DHW</t>
+  </si>
+  <si>
+    <t>Investment ST to DH</t>
+  </si>
+  <si>
+    <t>p_invest_ST2DH</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1088,6 +1094,17 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1099,7 +1116,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1454,7 +1471,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,13 +1574,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
connection cost to obj
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B922E7-CD95-479F-BFAB-CF7B7CD4BB63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069FE30-249D-446D-9E2F-FCDD61ED93EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -656,7 +656,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952F9C99-337E-41EB-9696-FC2C879F8079}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,7 +1471,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
variable cost to obj
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069FE30-249D-446D-9E2F-FCDD61ED93EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E76CB6-3A1F-4BF4-9F0F-D1CA58C89F2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,7 +1471,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added PV capacity and temperature factors
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E76CB6-3A1F-4BF4-9F0F-D1CA58C89F2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60207CF-0545-4BD9-8112-3EE48F35F6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
   <si>
     <t>PV</t>
   </si>
@@ -274,6 +274,72 @@
   </si>
   <si>
     <t>p_invest_ST2DH</t>
+  </si>
+  <si>
+    <t>Bonus shifting</t>
+  </si>
+  <si>
+    <t>p_shifting</t>
+  </si>
+  <si>
+    <t>PV to</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>Curtailment</t>
+  </si>
+  <si>
+    <t>ST to</t>
+  </si>
+  <si>
+    <t>Car to</t>
+  </si>
+  <si>
+    <t>Electric Grid to</t>
+  </si>
+  <si>
+    <t>Battery to</t>
+  </si>
+  <si>
+    <t>HP to</t>
+  </si>
+  <si>
+    <t>Irradiation STC</t>
+  </si>
+  <si>
+    <t>Irr_STC [kW/m²]</t>
+  </si>
+  <si>
+    <t>Temperatur factor PV</t>
+  </si>
+  <si>
+    <t>Performance ratio PV</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Surface Factor PV</t>
+  </si>
+  <si>
+    <t>30 grad, süd</t>
+  </si>
+  <si>
+    <t>Temperature STC</t>
+  </si>
+  <si>
+    <t>T_STC [°C]</t>
+  </si>
+  <si>
+    <t>[-%/°C]</t>
   </si>
 </sst>
 </file>
@@ -653,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,7 +735,7 @@
     <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -691,8 +757,26 @@
       <c r="G1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -714,8 +798,26 @@
       <c r="G2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -737,8 +839,17 @@
       <c r="G3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -757,8 +868,14 @@
       <c r="G4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -774,24 +891,36 @@
       <c r="G5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -799,42 +928,42 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -891,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,6 +1234,72 @@
         <v>100</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1115,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952F9C99-337E-41EB-9696-FC2C879F8079}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,13 +1666,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2019,7 +2215,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
all PV contraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60207CF-0545-4BD9-8112-3EE48F35F6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAF328E-5994-4BC5-9A56-6E38972E3931}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="104">
   <si>
     <t>PV</t>
   </si>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t>[-%/°C]</t>
+  </si>
+  <si>
+    <t>Efficiency ST</t>
+  </si>
+  <si>
+    <t>η_ST</t>
+  </si>
+  <si>
+    <t>Min Capacity PV Contractor</t>
+  </si>
+  <si>
+    <t>[kW]</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1298,6 +1310,28 @@
       </c>
       <c r="C24">
         <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all ST contraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAF328E-5994-4BC5-9A56-6E38972E3931}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB3A9B-C27B-422E-98F5-7AD9F20EB0E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="1160" yWindow="1220" windowWidth="14400" windowHeight="7370" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="106">
   <si>
     <t>PV</t>
   </si>
@@ -132,9 +132,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>P_ST_spec. [kW/pp]</t>
-  </si>
-  <si>
     <t>Reduction COP</t>
   </si>
   <si>
@@ -267,9 +264,6 @@
     <t>Demand</t>
   </si>
   <si>
-    <t>Specific DHW</t>
-  </si>
-  <si>
     <t>Investment ST to DH</t>
   </si>
   <si>
@@ -352,6 +346,41 @@
   </si>
   <si>
     <t>[kW]</t>
+  </si>
+  <si>
+    <t>Area ST per Person</t>
+  </si>
+  <si>
+    <r>
+      <t>A_ST_spec. [m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>²</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/pp]</t>
+    </r>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>Min Capacity ST Contractor</t>
   </si>
 </sst>
 </file>
@@ -361,7 +390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +409,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -749,43 +786,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
         <v>87</v>
-      </c>
-      <c r="K1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -793,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -805,13 +842,13 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -820,13 +857,13 @@
         <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -843,22 +880,22 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
         <v>81</v>
       </c>
-      <c r="I3" t="s">
-        <v>83</v>
-      </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -878,13 +915,13 @@
         <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -898,16 +935,16 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -915,7 +952,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
@@ -926,10 +963,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -937,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1032,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,13 +1087,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1072,7 +1109,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1105,21 +1142,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
       </c>
       <c r="C7">
         <v>0.45</v>
@@ -1127,10 +1164,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>70</v>
@@ -1138,10 +1175,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <v>22</v>
@@ -1149,10 +1186,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -1160,10 +1197,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>60</v>
@@ -1171,10 +1208,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>0.8</v>
@@ -1182,10 +1219,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>0.8</v>
@@ -1193,10 +1230,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1204,10 +1241,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -1215,10 +1252,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>60</v>
@@ -1226,10 +1263,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
       </c>
       <c r="C17">
         <v>0.2</v>
@@ -1237,10 +1274,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -1248,10 +1285,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19">
         <v>0.03</v>
@@ -1259,10 +1296,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1270,10 +1307,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21">
         <v>25</v>
@@ -1281,10 +1318,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22">
         <v>0.3</v>
@@ -1292,10 +1329,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23">
         <v>0.85</v>
@@ -1303,10 +1340,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24">
         <v>1.1000000000000001</v>
@@ -1314,10 +1351,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25">
         <v>0.75</v>
@@ -1325,12 +1362,23 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27">
         <v>2</v>
       </c>
     </row>
@@ -1359,7 +1407,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1368,7 +1416,7 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
@@ -1379,7 +1427,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1399,7 +1447,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1419,7 +1467,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1439,7 +1487,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1459,7 +1507,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1479,10 +1527,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
       </c>
       <c r="C7">
         <v>2000</v>
@@ -1499,10 +1547,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -1519,10 +1567,10 @@
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4">
         <v>1500</v>
@@ -1629,7 +1677,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <f ca="1">'Costs new investments'!C14*0.1</f>
@@ -1651,7 +1699,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <f ca="1">'Costs new investments'!C15*0.1</f>
@@ -1673,7 +1721,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <f ca="1">'Costs new investments'!C16*0.1</f>
@@ -1715,7 +1763,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
@@ -1724,7 +1772,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1816,19 +1864,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2261,13 +2309,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
all insulation constraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB3A9B-C27B-422E-98F5-7AD9F20EB0E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154B8BF9-A1E4-4C6A-A924-0ED1168E2F6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1220" windowWidth="14400" windowHeight="7370" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="1160" yWindow="1220" windowWidth="14400" windowHeight="7370" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
default heating constraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF30BB3-2332-4D05-AB76-583CB9FE5A29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCAD6CF-EEF2-4219-9087-E4EE52B5CBAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -774,7 +774,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
default HP constraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCAD6CF-EEF2-4219-9087-E4EE52B5CBAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8FF070-23EC-469E-ADB7-26C1CC5FB819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="109">
   <si>
     <t>PV</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>to Battery</t>
+  </si>
+  <si>
+    <t>to HP</t>
+  </si>
+  <si>
+    <t>Electric Grid</t>
   </si>
 </sst>
 </file>
@@ -771,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,7 +793,7 @@
     <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -830,8 +836,11 @@
       <c r="N1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -874,8 +883,11 @@
       <c r="N2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -907,10 +919,13 @@
         <v>81</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="O3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -939,7 +954,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -962,7 +977,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -973,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -984,7 +999,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -992,42 +1007,42 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1409,7 +1424,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,11 +1624,11 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f ca="1">'Costs new investments'!C10*0.1</f>
+        <f>C3*0.1</f>
         <v>150</v>
       </c>
       <c r="D10">
-        <f ca="1">'Costs new investments'!D10*1.2</f>
+        <f>D3*1.2</f>
         <v>240</v>
       </c>
       <c r="E10">
@@ -1631,11 +1646,11 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <f ca="1">'Costs new investments'!C11*0.1</f>
+        <f t="shared" ref="C11:C16" si="0">C4*0.1</f>
         <v>420</v>
       </c>
       <c r="D11">
-        <f ca="1">'Costs new investments'!D11*1.2</f>
+        <f t="shared" ref="D11:D16" si="1">D4*1.2</f>
         <v>240</v>
       </c>
       <c r="E11">
@@ -1653,11 +1668,11 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <f ca="1">'Costs new investments'!C12*0.1</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="D12">
-        <f ca="1">'Costs new investments'!D12*1.2</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E12">
@@ -1675,10 +1690,11 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <f ca="1">'Costs new investments'!C13*0.1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13">
@@ -1696,11 +1712,11 @@
         <v>63</v>
       </c>
       <c r="C14">
-        <f ca="1">'Costs new investments'!C14*0.1</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="D14">
-        <f ca="1">'Costs new investments'!D14*1.2</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E14">
@@ -1718,11 +1734,11 @@
         <v>64</v>
       </c>
       <c r="C15">
-        <f ca="1">'Costs new investments'!C15*0.1</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D15">
-        <f ca="1">'Costs new investments'!D15*1.2</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E15">
@@ -1740,11 +1756,11 @@
         <v>65</v>
       </c>
       <c r="C16">
-        <f ca="1">'Costs new investments'!C16*0.1</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D16">
-        <f ca="1">'Costs new investments'!D16*1.2</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E16">
@@ -1764,7 +1780,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Charging station constraints defines
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8FF070-23EC-469E-ADB7-26C1CC5FB819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A3EED9-4661-40B7-BC4C-639BD0169607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>PV</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>Electric Grid</t>
+  </si>
+  <si>
+    <t>to Car</t>
   </si>
 </sst>
 </file>
@@ -777,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,7 +796,7 @@
     <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -839,8 +842,11 @@
       <c r="O1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -886,8 +892,11 @@
       <c r="O2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -924,8 +933,11 @@
       <c r="O3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -953,8 +965,11 @@
       <c r="N4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -977,7 +992,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1007,42 +1022,42 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
all multi party house contraints defined
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A3EED9-4661-40B7-BC4C-639BD0169607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F19574-8B36-4CA2-A657-F2A452283C26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,6 +794,7 @@
     <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -831,10 +832,10 @@
         <v>84</v>
       </c>
       <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
         <v>86</v>
-      </c>
-      <c r="M1" t="s">
-        <v>87</v>
       </c>
       <c r="N1" t="s">
         <v>106</v>
@@ -843,7 +844,7 @@
         <v>107</v>
       </c>
       <c r="P1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -881,19 +882,19 @@
         <v>80</v>
       </c>
       <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>56</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>81</v>
-      </c>
-      <c r="N2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -927,13 +928,13 @@
       <c r="J3" t="s">
         <v>81</v>
       </c>
+      <c r="L3" t="s">
+        <v>108</v>
+      </c>
       <c r="N3" t="s">
         <v>108</v>
       </c>
       <c r="O3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -962,11 +963,11 @@
       <c r="J4" t="s">
         <v>56</v>
       </c>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
       <c r="N4" t="s">
         <v>56</v>
-      </c>
-      <c r="P4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
simple model workes with 24 timesteps
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A902C2C-9CBB-497B-8994-1989DC3DBEF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1D9E3A-BB94-419E-84DA-FEFB154BF726}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Demand" sheetId="13" r:id="rId5"/>
     <sheet name="Irradiation and temperatur" sheetId="15" r:id="rId6"/>
     <sheet name="irradiation_winter" sheetId="12" r:id="rId7"/>
+    <sheet name="Tabelle1" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="116">
   <si>
     <t>PV</t>
   </si>
@@ -396,6 +397,21 @@
   </si>
   <si>
     <t>Days</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>η_battery_gas</t>
+  </si>
+  <si>
+    <t>Thermal supply</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Electric supply</t>
   </si>
 </sst>
 </file>
@@ -786,7 +802,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K2" sqref="K2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1182,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1289,7 +1305,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1303,7 +1319,7 @@
         <v>72</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1448,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952F9C99-337E-41EB-9696-FC2C879F8079}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1805,7 +1821,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1909,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2345,11 +2361,25 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SUM(B2:B25)</f>
+        <v>88</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" ref="C26:E26" si="0">SUM(C2:C25)</f>
+        <v>90</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
@@ -2986,7 +3016,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3644,4 +3674,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98081729-F9A3-4045-8DF9-46396FFE460E}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <f>B6+B3</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10">
+        <f>B2+B5</f>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
electricity supply for household and car works
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1D9E3A-BB94-419E-84DA-FEFB154BF726}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D4C2A-7D22-456D-A161-7C86A6705BDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>η_battery_car</t>
   </si>
   <si>
-    <t>Number of household</t>
-  </si>
-  <si>
     <t>Simultaneity factor</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
   </si>
   <si>
     <t>Cost type default</t>
-  </si>
-  <si>
-    <t>Number of cars</t>
   </si>
   <si>
     <t>n_cars_total</t>
@@ -412,6 +406,12 @@
   </si>
   <si>
     <t>Electric supply</t>
+  </si>
+  <si>
+    <t>Number of Cars</t>
+  </si>
+  <si>
+    <t>Number of households</t>
   </si>
 </sst>
 </file>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,55 +818,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
         <v>83</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q1" t="s">
         <v>85</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" t="s">
-        <v>109</v>
-      </c>
-      <c r="N1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -877,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -889,13 +889,13 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -904,13 +904,13 @@
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" t="s">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -936,31 +936,31 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
         <v>79</v>
       </c>
-      <c r="J3" t="s">
-        <v>81</v>
-      </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -980,19 +980,19 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -1006,16 +1006,16 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -1023,7 +1023,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -1034,10 +1034,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
@@ -1045,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,13 +1159,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1181,7 +1181,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1198,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1214,10 +1214,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>1.5</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>37</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1313,21 +1313,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>60</v>
@@ -1335,10 +1335,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
       </c>
       <c r="C17">
         <v>0.2</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -1357,10 +1357,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19">
         <v>0.03</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1379,10 +1379,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21">
         <v>25</v>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>0.3</v>
@@ -1401,10 +1401,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>0.85</v>
@@ -1412,10 +1412,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24">
         <v>1.1000000000000001</v>
@@ -1423,10 +1423,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25">
         <v>0.75</v>
@@ -1434,24 +1434,24 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1488,7 +1488,7 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
       </c>
       <c r="C7">
         <v>2000</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>500</v>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="4">
         <v>1500</v>
@@ -1750,7 +1750,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1772,7 +1772,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -1794,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -1836,7 +1836,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
@@ -1845,7 +1845,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1925,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1937,19 +1937,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2362,7 +2362,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="2">
         <f>SUM(B2:B25)</f>
@@ -2732,10 +2732,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
@@ -3044,7 +3044,7 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -3680,8 +3680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98081729-F9A3-4045-8DF9-46396FFE460E}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3691,13 +3691,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -3723,7 +3723,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>82</v>
@@ -3744,7 +3744,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <f>B6+B3</f>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10">
         <f>B2+B5</f>

</xml_diff>

<commit_message>
HP and charging station capcity fixed
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D4C2A-7D22-456D-A161-7C86A6705BDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F018576-2D96-48D1-BC3B-2AB1BF30B2E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
   <si>
     <t>PV</t>
   </si>
@@ -391,9 +391,6 @@
   </si>
   <si>
     <t>Days</t>
-  </si>
-  <si>
-    <t>SUM</t>
   </si>
   <si>
     <t>η_battery_gas</t>
@@ -799,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,6 +923,9 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1131,6 +1131,126 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1143,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,7 +1318,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1305,7 +1425,7 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1313,7 +1433,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -1324,7 +1444,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
@@ -1465,7 +1585,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1925,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2361,186 +2481,412 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>109</v>
+      <c r="A26" s="2">
+        <v>25</v>
       </c>
       <c r="B26" s="2">
-        <f>SUM(B2:B25)</f>
-        <v>88</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" ref="C26:E26" si="0">SUM(C2:C25)</f>
-        <v>90</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>22</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>22</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
@@ -2717,10 +3063,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3002,6 +3348,270 @@
         <v>0</v>
       </c>
       <c r="C25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0.1002</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0.26207999999999998</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0.41768</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>0.55237000000000003</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>0.48031999999999997</v>
+      </c>
+      <c r="C35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0.60196000000000005</v>
+      </c>
+      <c r="C36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>0.48791000000000001</v>
+      </c>
+      <c r="C37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>0.27662999999999999</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>0.19836000000000001</v>
+      </c>
+      <c r="C39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>0.25089</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>0.21872999999999998</v>
+      </c>
+      <c r="C41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>7.6659999999999992E-2</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6.1600000000000005E-3</v>
+      </c>
+      <c r="C43">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
         <v>15</v>
       </c>
     </row>
@@ -3691,7 +4301,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -3744,7 +4354,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9">
         <f>B6+B3</f>
@@ -3753,7 +4363,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10">
         <f>B2+B5</f>

</xml_diff>

<commit_message>
changed supply_to_ var to 3 index
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F018576-2D96-48D1-BC3B-2AB1BF30B2E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0728C5B-E81B-4894-B4F5-49783417881E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
@@ -799,7 +799,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,7 +1373,7 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1384,7 +1384,7 @@
         <v>35</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2043,10 +2043,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2366,7 +2366,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -2383,7 +2383,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -2400,7 +2400,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -2417,7 +2417,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -2774,7 +2774,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>5</v>
@@ -2791,7 +2791,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -2808,7 +2808,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -2825,7 +2825,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -3048,13 +3048,6 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3065,13 +3058,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
supply from car has no index finance option anymore
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0728C5B-E81B-4894-B4F5-49783417881E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C29EC8B-2847-48F5-AFB2-A0C87FA3DF89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -796,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,10 +868,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>62</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -1050,206 +1050,211 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
     </row>
@@ -1263,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1439,7 +1444,7 @@
         <v>70</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1585,7 +1590,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2043,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2074,9 +2079,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
@@ -2091,7 +2096,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -2108,7 +2113,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -2125,7 +2130,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -2142,7 +2147,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2159,24 +2164,24 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -2193,7 +2198,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -2210,7 +2215,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -2227,7 +2232,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -2244,7 +2249,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -2261,7 +2266,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -2278,7 +2283,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -2295,7 +2300,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -2312,7 +2317,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -2329,7 +2334,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -2346,7 +2351,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -2363,7 +2368,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
@@ -2380,10 +2385,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -2397,10 +2402,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -2414,10 +2419,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -2431,7 +2436,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -2448,7 +2453,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -2465,24 +2470,24 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -2499,7 +2504,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
@@ -2516,7 +2521,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -2533,7 +2538,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -2550,7 +2555,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -2567,24 +2572,24 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -2601,7 +2606,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -2618,7 +2623,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -2635,7 +2640,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -2652,7 +2657,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -2669,7 +2674,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
         <v>0</v>
@@ -2686,7 +2691,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>0</v>
@@ -2703,7 +2708,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2">
         <v>0</v>
@@ -2720,7 +2725,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2">
         <v>0</v>
@@ -2737,7 +2742,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2">
         <v>0</v>
@@ -2754,7 +2759,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2">
         <v>0</v>
@@ -2771,7 +2776,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>0</v>
@@ -2788,10 +2793,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -2805,10 +2810,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -2822,10 +2827,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -2839,7 +2844,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2">
         <v>0</v>
@@ -2856,7 +2861,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2">
         <v>0</v>
@@ -2873,27 +2878,37 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
@@ -3048,6 +3063,13 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3056,10 +3078,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3082,7 +3104,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3093,7 +3115,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3104,7 +3126,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3115,7 +3137,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3126,21 +3148,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1002</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -3148,10 +3170,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.26207999999999998</v>
+        <v>0.1002</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -3159,10 +3181,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0.41768</v>
+        <v>0.26207999999999998</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -3170,10 +3192,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>0.55237000000000003</v>
+        <v>0.41768</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -3181,21 +3203,21 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>0.48031999999999997</v>
+        <v>0.55237000000000003</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>0.60196000000000005</v>
+        <v>0.48031999999999997</v>
       </c>
       <c r="C12">
         <v>17</v>
@@ -3203,21 +3225,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>0.48791000000000001</v>
+        <v>0.60196000000000005</v>
       </c>
       <c r="C13">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>0.27662999999999999</v>
+        <v>0.48791000000000001</v>
       </c>
       <c r="C14">
         <v>18</v>
@@ -3225,21 +3247,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>0.19836000000000001</v>
+        <v>0.27662999999999999</v>
       </c>
       <c r="C15">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>0.25089</v>
+        <v>0.19836000000000001</v>
       </c>
       <c r="C16">
         <v>19</v>
@@ -3247,10 +3269,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>0.21872999999999998</v>
+        <v>0.25089</v>
       </c>
       <c r="C17">
         <v>19</v>
@@ -3258,10 +3280,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>7.6659999999999992E-2</v>
+        <v>0.21872999999999998</v>
       </c>
       <c r="C18">
         <v>19</v>
@@ -3269,29 +3291,29 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>6.1600000000000005E-3</v>
+        <v>7.6659999999999992E-2</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>6.1600000000000005E-3</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3302,18 +3324,18 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3324,7 +3346,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3335,7 +3357,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3346,7 +3368,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3357,7 +3379,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3368,7 +3390,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3379,7 +3401,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3390,21 +3412,21 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>0.1002</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -3412,10 +3434,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>0.26207999999999998</v>
+        <v>0.1002</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -3423,10 +3445,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>0.41768</v>
+        <v>0.26207999999999998</v>
       </c>
       <c r="C33">
         <v>16</v>
@@ -3434,10 +3456,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>0.55237000000000003</v>
+        <v>0.41768</v>
       </c>
       <c r="C34">
         <v>16</v>
@@ -3445,21 +3467,21 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>0.48031999999999997</v>
+        <v>0.55237000000000003</v>
       </c>
       <c r="C35">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>0.60196000000000005</v>
+        <v>0.48031999999999997</v>
       </c>
       <c r="C36">
         <v>17</v>
@@ -3467,21 +3489,21 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>0.48791000000000001</v>
+        <v>0.60196000000000005</v>
       </c>
       <c r="C37">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>0.27662999999999999</v>
+        <v>0.48791000000000001</v>
       </c>
       <c r="C38">
         <v>18</v>
@@ -3489,21 +3511,21 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>0.19836000000000001</v>
+        <v>0.27662999999999999</v>
       </c>
       <c r="C39">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>0.25089</v>
+        <v>0.19836000000000001</v>
       </c>
       <c r="C40">
         <v>19</v>
@@ -3511,10 +3533,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>0.21872999999999998</v>
+        <v>0.25089</v>
       </c>
       <c r="C41">
         <v>19</v>
@@ -3522,10 +3544,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>7.6659999999999992E-2</v>
+        <v>0.21872999999999998</v>
       </c>
       <c r="C42">
         <v>19</v>
@@ -3533,29 +3555,29 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>6.1600000000000005E-3</v>
+        <v>7.6659999999999992E-2</v>
       </c>
       <c r="C43">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>6.1600000000000005E-3</v>
       </c>
       <c r="C44">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -3566,18 +3588,18 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -3588,7 +3610,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -3599,12 +3621,23 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added binary for up and down shift
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43C6198-1153-4DB0-B6B0-AD98360381CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267BFFD5-4C75-4411-9229-3D544139D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" firstSheet="2" activeTab="5" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="117">
   <si>
     <t>PV</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>kW</t>
-  </si>
-  <si>
-    <t>&lt;&lt;</t>
   </si>
 </sst>
 </file>
@@ -819,6 +816,7 @@
     <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1154,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1242,7 +1240,7 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>0.45</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1374,7 +1372,7 @@
         <v>75</v>
       </c>
       <c r="C19">
-        <v>0.03</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1487,7 +1485,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1698,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1731,8 +1729,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
@@ -1842,7 +1839,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1897,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0.1</v>
@@ -1944,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1956,7 +1953,7 @@
     <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1973,7 +1970,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2007,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2024,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2041,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2058,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2066,16 +2063,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2089,10 +2086,10 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2106,10 +2103,10 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2123,10 +2120,10 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2140,10 +2137,10 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2151,16 +2148,16 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2168,16 +2165,16 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2185,19 +2182,16 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2205,16 +2199,16 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2222,13 +2216,13 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2239,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2256,13 +2250,13 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2273,13 +2267,13 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>5</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2296,7 +2290,7 @@
         <v>5</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2313,7 +2307,7 @@
         <v>5</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2330,7 +2324,7 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -2347,7 +2341,7 @@
         <v>5</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -2358,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -2375,13 +2369,13 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2403,7 +2397,6 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
@@ -2500,9 +2493,6 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
@@ -2667,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3046,8 +3036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
capacities and supply shown by visualisation
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267BFFD5-4C75-4411-9229-3D544139D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC3DF47-BC63-4D0E-97BA-5CF4C0A517E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" firstSheet="2" activeTab="5" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1838,7 +1838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429933C5-DFD0-42DC-9288-AD78420EFB5D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1894,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="E3">
         <v>0.1</v>
@@ -2657,7 +2657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed from connection capacity to big M (Gas/DH constraint)
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47FFF67-39E1-4070-94CD-6022D5EF3768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A882C9-DC3C-4FB6-B368-43E3AB750B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -802,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -930,6 +930,9 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1140,6 +1143,126 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1150,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1166,7 +1289,7 @@
     <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1177,7 +1300,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1311,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1198,8 +1321,12 @@
       <c r="C3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f>((1+C2)^C3)*C2/((1+C2)^C3-1)</f>
+        <v>7.7825472250244179E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1337,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1221,7 +1348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1232,7 +1359,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1243,7 +1370,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1254,7 +1381,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1265,7 +1392,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1276,7 +1403,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1287,7 +1414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1298,7 +1425,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1309,7 +1436,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1320,7 +1447,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -1331,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -1485,7 +1612,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C16"/>
+      <selection activeCell="C3" sqref="C3:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -1565,7 +1692,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>4200</v>
       </c>
       <c r="D4">
         <v>200</v>
@@ -1585,7 +1712,7 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>550</v>
       </c>
       <c r="D5">
         <v>200</v>
@@ -1605,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1625,7 +1752,7 @@
         <v>62</v>
       </c>
       <c r="C7">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -1645,7 +1772,7 @@
         <v>63</v>
       </c>
       <c r="C8">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D8">
         <v>200</v>
@@ -1664,8 +1791,8 @@
       <c r="B9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C9">
-        <v>200</v>
+      <c r="C9" s="4">
+        <v>1500</v>
       </c>
       <c r="D9" s="4">
         <v>200</v>
@@ -1685,7 +1812,8 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>200</v>
+        <f>C3*0.1</f>
+        <v>150</v>
       </c>
       <c r="D10">
         <f>D3*1.2</f>
@@ -1706,10 +1834,11 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>200</v>
+        <f t="shared" ref="C11:C16" si="0">C4*0.1</f>
+        <v>420</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D15" si="0">D4*1.2</f>
+        <f t="shared" ref="D11:D15" si="1">D4*1.2</f>
         <v>240</v>
       </c>
       <c r="E11">
@@ -1727,10 +1856,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E12">
@@ -1748,10 +1877,11 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13">
@@ -1769,10 +1899,11 @@
         <v>62</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E14">
@@ -1790,10 +1921,11 @@
         <v>63</v>
       </c>
       <c r="C15">
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="E15">
@@ -1811,7 +1943,8 @@
         <v>64</v>
       </c>
       <c r="C16">
-        <v>200</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="D16">
         <v>360</v>
@@ -1833,7 +1966,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B3" sqref="B3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1908,7 +2041,7 @@
         <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1937,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDCAAEF-9BC9-4D67-B5C1-5585BDAAB9DD}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E26"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="B51:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2390,99 +2523,412 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2">
+        <v>22</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2">
+        <v>22</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
@@ -2651,8 +3097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D891D-3F2A-4DCE-83B8-FA3AAFA767F2}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2949,76 +3395,268 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0.1002</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0.26207999999999998</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.41768</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.55237000000000003</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.48031999999999997</v>
+      </c>
+      <c r="C36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.60196000000000005</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.48791000000000001</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.27662999999999999</v>
+      </c>
+      <c r="C39">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0.19836000000000001</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.25089</v>
+      </c>
+      <c r="C41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0.21872999999999998</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>7.6659999999999992E-2</v>
+      </c>
+      <c r="C43">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>6.1600000000000005E-3</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3030,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95034383-FE85-4F68-924D-0BEBCE2AD864}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7:G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>